<commit_message>
updated bom with pot
</commit_message>
<xml_diff>
--- a/pcb/logic/bom.xlsx
+++ b/pcb/logic/bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Projects\coincidenceCounter\pcb\logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>QTY</t>
   </si>
@@ -134,9 +134,6 @@
     <t>0R Jumper</t>
   </si>
   <si>
-    <t>R2, R3, R5, R8, R10</t>
-  </si>
-  <si>
     <t>Standoffs</t>
   </si>
   <si>
@@ -252,6 +249,27 @@
   </si>
   <si>
     <t>3/16" Hex Size, 1/4" Length, 4-40 Thread Size</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>TRIMMER 10K OHM 0.25W SMD</t>
+  </si>
+  <si>
+    <t>3314Z-1-103E</t>
+  </si>
+  <si>
+    <t>3314Z-103ECT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/bourns-inc/3314Z-1-103E/3314Z-103ECT-ND/253541</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R2, R3, R5</t>
   </si>
 </sst>
 </file>
@@ -262,7 +280,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +329,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -334,7 +358,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -348,6 +372,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,14 +663,14 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
@@ -690,16 +718,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="F2" s="7">
         <v>2</v>
@@ -708,13 +736,13 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" s="5">
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -722,13 +750,13 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F3" s="7">
         <v>3</v>
@@ -737,13 +765,13 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="5">
         <v>1.11E-2</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -754,13 +782,13 @@
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
@@ -769,42 +797,42 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="5">
-        <v>1.8499999999999999E-2</v>
+        <v>1.11E-2</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -812,7 +840,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
@@ -844,7 +872,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -862,7 +890,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="5">
         <v>0.20499999999999999</v>
@@ -876,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -908,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -926,7 +954,7 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="5">
         <v>0.35199999999999998</v>
@@ -935,21 +963,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F10" s="2">
         <v>4</v>
@@ -958,13 +986,13 @@
         <v>0.36</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I10" s="5">
         <v>1.44</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -972,16 +1000,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
@@ -990,30 +1018,30 @@
         <v>1.835</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I11" s="5">
         <v>1.835</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1022,18 +1050,46 @@
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="5">
         <v>0</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="2"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="5">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>

</xml_diff>